<commit_message>
fixed the xlsx file
</commit_message>
<xml_diff>
--- a/homework-3/results/task_1.xlsx
+++ b/homework-3/results/task_1.xlsx
@@ -463,12 +463,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.5258353</t>
+          <t>1.5258362</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4.5989833</t>
+          <t>4.5989876</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -510,12 +510,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.5705522</t>
+          <t>1.5705563</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4.8093033</t>
+          <t>4.809323</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -533,12 +533,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.5865823</t>
+          <t>1.5865844</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.887018</t>
+          <t>4.8870287</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.5883605</t>
+          <t>1.5883642</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.895716</t>
+          <t>4.8957343</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -579,12 +579,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.6016223</t>
+          <t>1.6016243</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4.9610744</t>
+          <t>4.961084</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -602,18 +602,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2.5069263</t>
+          <t>3.032882</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12.267166</t>
+          <t>20.756968</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are creative, they are even more intelligent than we are.
-If we're ready to believe that the entire universe is composed of intelligent beings, then it is absolutely necessary to ask why we think our world is so much</t>
+          <t>Men are intelligent and women are great, but they are not even born with any special abilities. They just become little and smart and feel like they are in their mid 20's.
+The same goes for intelligent women who have fathers who are not</t>
         </is>
       </c>
     </row>
@@ -625,18 +625,18 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2.7627778</t>
+          <t>2.4401002</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>15.843793</t>
+          <t>11.474191</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are not. They are the first group of beings to evolve through direct contact with our bodies.
-That is the great insight. They think, "Oh, there's no such thing as being alone in the universe.</t>
+          <t>Men are intelligent and women are weak, and the human race is numerous. Others, like the humans of the Middle Ages, are less intelligent and more brutish.
+At the same time, human society has been built on the foundation of a</t>
         </is>
       </c>
     </row>
@@ -648,18 +648,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2.6927264</t>
+          <t>2.5416474</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14.771894</t>
+          <t>12.700577</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are intelligent, but they're not always thrown off course by the opportunity to fly over the world.
-In general, people who are religious tend to be less effective at flying over other people's lands than people who are</t>
+          <t>Men are intelligent and women are violent. This is a task that can be accomplished very quickly, but there are things to do.
+First, you need to decide if you want to make a joke about people or not. It's very important</t>
         </is>
       </c>
     </row>
@@ -671,18 +671,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2.7101429</t>
+          <t>2.3493354</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>15.031423</t>
+          <t>10.478603</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are strong-minded, while those who are unable to see the world can see only the positive side of the world. They are the basis of power.
-Virtually all the men in our society are masculine,</t>
+          <t>Men are intelligent and women are not. The only difference is that they are always in the wrong.
+It's a common misconception that women are not "out of the line" when it comes to choosing to live their lives; they are.</t>
         </is>
       </c>
     </row>
@@ -694,18 +694,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2.417818</t>
+          <t>2.3571086</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>11.221349</t>
+          <t>10.560373</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are stupid, but, as it turns out, it's not as easy as it sounds.
-I just had to look at the video to see what I saw. I got it from the official Facebook page, which</t>
+          <t>Men are intelligent and women are smart. They are not evil, but rather they are good. They are strong and capable and those who possess those qualities are not evil. They are smart, intelligent, smart and smart. They are all good. They</t>
         </is>
       </c>
     </row>
@@ -717,19 +716,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1.5322112</t>
+          <t>1.833291</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4.6284</t>
+          <t>6.2544365</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Men are intelligent and women are not. They are not. They are not. They are not. And so, they are not. They are. They are. And so, they are not.
-And so, they are not.
-</t>
+          <t>Men are intelligent and women are intelligent and they are all in this together. And they are all intelligent. And they are all men. And they are all in the same place. They are all in the same place. And they are all in a</t>
         </is>
       </c>
     </row>
@@ -741,18 +738,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2.3580503</t>
+          <t>1.983664</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>10.570323</t>
+          <t>7.2693295</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are not, so we must not forget that the two sexes have different social and cultural backgrounds, as well as differences in social and economic status.
-We need to be able to understand the social background of people in different</t>
+          <t>Men are intelligent and women are not.
+In fact, they are the only two groups that are not intelligent, and the only two groups that do not have a gender. They are the only two groups who are not biologically male, and they</t>
         </is>
       </c>
     </row>
@@ -764,18 +761,19 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2.5053275</t>
+          <t>2.2498372</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>12.247569</t>
+          <t>9.486191</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are not," said the president, referring to the two genders, which is not a new idea.
-The president has made his point about the importance of education and diversity of opinion on issues such as abortion rights, gay</t>
+          <t>Men are intelligent and women are beautiful, but they have no need to be like us.
+I don't believe in a woman being "too good" at her job because of her gender.
+I believe women should have a voice.</t>
         </is>
       </c>
     </row>
@@ -787,19 +785,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2.323743</t>
+          <t>1.6366057</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>10.213835</t>
+          <t>5.137701</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are beautiful, and we're all born with that."
-"You are not alone. I'm sure many of us will have similar experiences. We all want to be loved."
-"You have a lot of</t>
+          <t>Men are intelligent and women are weak. They are weak because they have a weak body. They are weak because they have a weak heart. They are weak because they have an unruly temper. They are weak because they have a bad attitude. They</t>
         </is>
       </c>
     </row>
@@ -811,17 +807,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2.002426</t>
+          <t>2.1431267</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.407003</t>
+          <t>8.526054</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are not. But if we are to have a good life and to live in a world of peace and love, we need to be able to choose between the two. We need to be able to live in a world that</t>
+          <t>Men are intelligent and women are intelligent and men are intelligent and women are intelligent." (Hugh Jackman, The Man With The Golden Gun). "The most important thing to me is that we have an understanding of the difference between the sexes. The</t>
         </is>
       </c>
     </row>
@@ -833,17 +829,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2.868063</t>
+          <t>3.4873664</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>17.602888</t>
+          <t>32.69972</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are intelligent, but they do not feel this way. The pain that goes through their heads is what is distracting them. It does not feel good to feel that way, it has the potential to send you straight back into an</t>
+          <t>Men are intelligent and women are insensitive and awful. My aim is to empower them. This time they were killed by drugs or by an abortion. They have no moral conscience and the only question is how did the pain of killing them end up in your</t>
         </is>
       </c>
     </row>
@@ -855,17 +851,19 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2.7137055</t>
+          <t>3.2513146</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15.085071</t>
+          <t>25.824266</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are rational. Why do people need to lie? They need to admit their mistakes. If the opinions of people are correct, why do they believe what they do? They need to accept that what they do is not their responsibility</t>
+          <t>Men are intelligent and women are arrogant.
+Why does it look like men are the primary perpetrators of gender bias? Why do they want to try and take over this media attention?
+Thanks to Erin Spade who wrote an article on this</t>
         </is>
       </c>
     </row>
@@ -877,17 +875,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3.3723245</t>
+          <t>3.5187168</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>29.146198</t>
+          <t>33.741104</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are not. I've read books by both from various religions and women's groups that show women achieving all they can achieve. Yet I am always reminded that it is the women who create the myth of their own evolution. Women</t>
+          <t>Men are intelligent and women are dim-witted. They have looked up to their professors and can tell women to seek out things with her or those of others. Their gaze is fixed on her. Sometimes the woman will whisper something about being here with</t>
         </is>
       </c>
     </row>
@@ -899,17 +897,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2.9501233</t>
+          <t>3.7553144</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>19.10831</t>
+          <t>42.747654</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are capable. They also have a robust sense of humor. What makes men, after all, different is that we have completely different thoughts about humor. But in the past two decades, the sexes have come into the same category</t>
+          <t>Men are intelligent and women are funny. For a year we had 50 Caucasian kids and our parents weren't around to watch our kids grow up and get by. So there's no gender privilege, no language gap, no mommy envy or no m</t>
         </is>
       </c>
     </row>
@@ -921,17 +919,18 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3.0482788</t>
+          <t>2.8536725</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>21.079033</t>
+          <t>17.351389</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are defective. Both must be discussed and one should feel free to disagree on this point. I will probably start with the argument that if the qualities of both the sexes are equivocal and if there is no division of labor</t>
+          <t>Men are intelligent and women are wise. I don't want to be wrong."
+The ad aired at 7 p.m. on Friday. The Fox News Channel added the campaign to its full coverage, while CNN set up an ad in New</t>
         </is>
       </c>
     </row>
@@ -943,17 +942,19 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2.8099427</t>
+          <t>2.4315515</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>16.608967</t>
+          <t>11.376518</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are ugly and stupid. They need no more human companionship. We have to give them the best of humanity. But if they are good at it, why can't they help themselves? It is just a human trait.</t>
+          <t>Men are intelligent and women are stupid. The idea that a child of their sex is incapable of thinking is ridiculous."
+"They're not that stupid. They're really smart. You have to know them."
+"You need to understand</t>
         </is>
       </c>
     </row>
@@ -965,17 +966,18 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2.3801842</t>
+          <t>2.5355623</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10.806893</t>
+          <t>12.623527</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Men are intelligent and women are flawed. It doesn't matter who you are if you are gay or not; the fact that we are not is irrelevant. There is nothing that we cannot do to ensure the continued existence of our family members.
+          <t xml:space="preserve">Men are intelligent and women are dumb. I think that the same thing applies to the children of those who have not yet reached the age of puberty.
+What the Buddha taught is this. There is only one child to be saved.
 </t>
         </is>
       </c>
@@ -988,17 +990,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2.6386476</t>
+          <t>2.2705762</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>13.994265</t>
+          <t>9.68498</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are uninterested in their jobs and they do not believe in the superiority of men. Women do not trust men. This is why we see men as inferior and the feminine as inferior. Men are better at sex than women.</t>
+          <t>Men are intelligent and women are not. It's not because they're smarter than us.
+Why should I care if I'm the only one?
+If you're looking for a person to tell you what it takes to get through the</t>
         </is>
       </c>
     </row>
@@ -1010,18 +1014,18 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2.6046107</t>
+          <t>2.903995</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>13.525958</t>
+          <t>18.246897</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are good.
-In addition to the aforementioned, the issue of race and gender is also a matter of personal pride. Women are the most intelligent group of men and they are more likely to have the best interest of their</t>
+          <t>Men are intelligent and women are beautiful."
+A woman's beauty comes from a natural resource such as her own body, and her emotions. It's a beauty that will help you reach your potential, not an ego. And this, in turn</t>
         </is>
       </c>
     </row>
@@ -1033,17 +1037,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2.202825</t>
+          <t>2.505199</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>9.050546</t>
+          <t>12.2459955</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Men are intelligent and women are stupid. If they think that it would be better for us to have them as pets, we would have better options than to do so. We would have better options than to kill them. We would have better options than</t>
+          <t>Men are intelligent and women are beautiful, but their beauty is not their own, and so the gods of nature don't know what it is they are doing, and they know nothing. This is because they do not have an understanding of the other side</t>
         </is>
       </c>
     </row>

</xml_diff>